<commit_message>
Get daily reddit data: Tue Mar 19 08:07:56 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_24.xlsx
+++ b/data/2024_03_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C427"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2149 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1bieshb</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>The Macro image shows everything 🤩</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8u56fpqw8pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1biera2</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Hand painted 🖤🩵🤍</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1biera2</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1biemm6</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Should I do dip or acrylic overlay on my natural nails?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1biemm6/should_i_do_dip_or_acrylic_overlay_on_my_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1biejl3</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>2nd set!!</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7tk27rit8pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1bicyjt</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>New to getting nails done and had questions</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bicyjt</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1bicxmi</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Longest natural length I’ve had</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bicxmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1bibdcq</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>I have ONE nail where the gel keeps coming off in one peel</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bibdcq/i_have_one_nail_where_the_gel_keeps_coming_off_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1bibug7</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Do you like almond or oval more?</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bibug7</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1bi650r</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>did these nails on a client yesterday, what do we think?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi650r</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1biadp6</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Freehand tarot eye. Been working on my line work. What do you think?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqmooxl7k7pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1biacwn</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>a few press on nails i’ve done recently! :,)</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1biacwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1bi9b4y</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Beetles clear builder gel and pastels</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi9b4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1bi7no5</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Flower 🌼 </t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwlzt89ww6pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1bi7fp4</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Oil spills? Foils did me dirty ⭐️🌚</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi7fp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1bi7bfs</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>St Patrick's Day a wee bit late</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi7bfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1bi6uhk</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>💜💛</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tfrx4h3hq6pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1bi6ofj</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Does a real no-chip top coat exist for basic nail polish?</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bi6ofj/does_a_real_nochip_top_coat_exist_for_basic_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1bi3x7w</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>I asked for gel nails and she just gave me nail polish—-I’m really confused?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/revnnscn46pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1bi4rq8</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>First manicure/acrylics/first time I’m willing to show my hands to the world.</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ntbmj5qwa6pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1bi6bn7</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Fresh Nails</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gj8qxxaem6pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1bi686r</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Chrome stars</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi686r</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1bi64z6</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first soft gel nails. Constructive criticism😄🫶🏻
+</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ri4li80l6pc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1bi5hjj</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Mermaid Marble</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0i5mdx5g6pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1bi5dy3</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>I’m a dip powder convert!</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/982ny4kff6pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1bi4kw9</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>what happend?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pitqg21i96pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1bi4kbf</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Nails of the week 💅🏽 Glossy vs Matte</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi4kbf</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1bi1n4t</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Fox nails</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7ypocgno5pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1bi1i8f</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Tips for doing your own gel nails?</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bi1i8f/tips_for_doing_your_own_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1bi18u7</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>I’ve been using hard as hoof to grow out my nails and I’m using cuticle oil too but one of my nails looks like it will split in the middle at some point…</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi18u7</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1bhxe6v</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>How do I go about finding a nail salo?.</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bhxe6v/how_do_i_go_about_finding_a_nail_salo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1bi085m</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nothing special just a rainbow design I did </t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/053fmk7qe5pc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1bhzrjb</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Love my nails</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4loat9e9b5pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1bhy73u</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can I get good French tips with the nail art tools? </t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bhy73u/how_can_i_get_good_french_tips_with_the_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1bhy60x</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Subtle Nails</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgemm26605pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1bhxy4b</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Do you like it?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhxy4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1bhxna3</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Spring is in the air 🎀</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rlx02x1hw4pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1bhxj1y</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Yellow may not be everyone’s cup of tea but it’s mine!</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwh34scnv4pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1bhxina</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Bit late but 🍀Happy St.Patrick's day 🍀</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7c5wb0jv4pc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1bhxcix</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Oranges and French tip because I’m ready for summer🍊🥰</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhxcix</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1bhwzn0</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>What you guys think?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhwzn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1bhwyfn</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Artist slayed once again ✨</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jlldf0nr4pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1bhwiom</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Is this color too warm for me?</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eoqbwhego4pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1bhw4s9</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IDK why nails NEVER last for me </t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bhw4s9/idk_why_nails_never_last_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1bhvtvq</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it normal for the start of the whites to be yellow/transparent? </t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jcyp6u1ij4pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1bhvoga</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Girls' day out at the nail salon</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjrqmb9hi4pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1bhrs30</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matte top coat </t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bhrs30/matte_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1bhufpz</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Essie's Sheer Fantasy 💅🏻 my favorite sheer pink so far</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhufpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1bhn8py</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>gel matte topcoat</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bhn8py/gel_matte_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1bhtqcr</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>These look decent?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhtqcr</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1bhtq18</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Second time doing gel nails!</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5qkemcb44pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1bhtcxe</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Criticism welcome </t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2vcukiyi14pc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1bhbuk0</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>I know there bad but if you saw them in person what would be your reaction or thought… I know my hand lol they where still drying</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4982y7yw8zoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1bhsw1y</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Help! I broke a nail</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/121an09yx3pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1bhss8q</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>From last January 🥰</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eujzpuj7x3pc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1bhsqwx</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Princess nails for my birthday!</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrbxqgyxw3pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1bhsqp9</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Last set before I try polygel!</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcbc38cww3pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1bhsbuj</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Kiss press ons + chrome powder 🤍</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhsbuj</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1bhs96s</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Deco Flower Nails!! (Home done, no certificate)</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhs96s</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1bhr9da</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t xml:space="preserve">you guysss!!!! I‘m obsessed </t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f63m65eil3pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1bhpek7</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Spring Nails ☺️</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7igim5cb53pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1bhosif</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Kiss press ons 🤌💅</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmjt746fz2pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1bhn610</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>First time getting gel polish, I love it! 🥰</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/se39wjoih2pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1bhmg1k</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question for my long nails girlies </t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bhmg1k/question_for_my_long_nails_girlies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1bhm61i</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Tried to do mermaid nails</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhm61i</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1bidm02</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Galaxy nails </t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nztlqpiqh8pc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1bid23q</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Continued adventures in chrome powder with regular nail polish (instructions in comments) </t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/noyrtwm5b8pc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1bicy9p</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>St. Patrick's Day nails that I didn't actually get to wear on St. Patrick's Day</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oa5ipadm98pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1bicd8t</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Is crazy what a high quality primer, nail polish, and top coat do! First pic is freshly painted, second is 11 days later. My polish used to chip the next day. Just like a gel manicure</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bicd8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1bic67p</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Try a lil Pink</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bic67p</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1bibp9s</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m so happy I grabbed Lemon by Bees Knees Lacquer. </t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1itykuhw7pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1bibo6f</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Went a little crazy for bluey-greens/greenish-blues…</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bibo6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1bibkxb</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Can anyone help me find something similar to Polished For Days "Violet Prism"?</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bibkxb/can_anyone_help_me_find_something_similar_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1bibdpg</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Had no time to tidy up, hands were dry, but here's Take the Leap from Sweet &amp; Sour Lacquer!</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1a9y8bict7pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1bib82j</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It’s come to my attention that some people have issues with my swatching photos. </t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bib82j/its_come_to_my_attention_that_some_people_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1bi8li0</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Any Hazbin hotel fans?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi8li0</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1bi8igd</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Any Dupes for OPI “I’m Yatch Leaving”?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bi8igd/any_dupes_for_opi_im_yatch_leaving/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1bi7m9u</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Delayed posting of my St Patrick’s Day mani - now to put this polish away until next year or when I can afford a holiday to Ireland! Application inspected and approved by Bono (17M Tabby/Maine Coon x)</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi7m9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1bi7cce</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>St Patrick's Day fun</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi7cce</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1bi6ykj</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Replacement Clionadh Brushes</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bi6ykj/replacement_clionadh_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1bi6j9b</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Boolba layered over China Glaze Treble Maker</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi6j9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1bi5qf9</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Deep green 💚</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k562i3uxh6pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1bi505q</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>St. Patrick’s Day mani 🍀</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi505q</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1bi4xvi</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Mondays are the worst 😭</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi4xvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1bi49mi</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Where to find this specific swatch stick</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2693qzr676pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1bi3rz3</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Milk Chocolate 🍫</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi3rz3</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1bi3bqj</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Some Updates</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bi3bqj/some_updates/</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1bhyakd</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Mooncat House of Hades</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhyakd</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1bi0xgr</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>St Patty’s Day mani matches my drink 😂</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fp6e9w7nj5pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1bi0t3z</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>🧡Clown Fish🧡</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi0t3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1bi0rl5</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Love a luscious lacquer</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bi0rl5</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1bhzvqn</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Constellation</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bhzvqn/constellation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1bhzfzd</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Mooncat "Eternal Sunshine" with Orly "What's The Big Teal"</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4tnbqqr85pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1bhywrr</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Cozen by LynBDesigns feeling more green than I expected but I dig it</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6e5t5jqf55pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1bhymkh</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Color me impressed</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhymkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1bhy42u</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>ILNP “First Snow”</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhy42u</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1bhy3ka</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>An unusual request</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bhy3ka/an_unusual_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1bhxkxk</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Red Shorties</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6okm5x0w4pc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1bhwule</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>After much experimentation, my first DIY jelly polish is a success! 🥰</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhwule</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1bhws00</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>The goal was disco ball ballerina</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8g88p14cq4pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1bhwiys</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Does anybody else have a palate cleanser shade that isn’t really a palate cleanser?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdi05j6ho4pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1bhw0cb</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>GOSH Holographic - my beloved</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhw0cb</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1bhvey6</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Lyn B Thermal 🔥</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhvey6</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1bhujir</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Nails looking rough after using Essie gel couture?</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nr73ww8a4pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1bhsh5a</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Cirque Colors Lucky Jelly ♥️</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhsh5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1bhu4xi</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Cuticle Oil is not an option while at work</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bhu4xi/cuticle_oil_is_not_an_option_while_at_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1bhs0kl</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Did someone say green?</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhs0kl</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1bhsufk</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>LynB- Tenta Cool</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e035i37mx3pc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1bhssy2</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Morningtide is so pretty</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thcstjxbx3pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1bhsq7g</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Cirque is bringing back Coronation again</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nriwtbosw3pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1bhsa5h</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Lumen Snow Shadow</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bhsa5h/lumen_snow_shadow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1bhrvfz</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>couldn’t resist being a part of the photos! he must know how perfectly his eyes match jade jelly 😻</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhrvfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1bhruz5</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Nails inc ‘check please’ skittles</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhnbq0d5q3pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1bhqv4f</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>I did some layering</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ezi19re4i3pc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1bhqm55</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Enchantment 🧚‍♂️</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhqm55</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1bhpjwe</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Pink Gellac colors</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bhpjwe/pink_gellac_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1bhoyj0</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Looks like sequins in the right lighting ✨</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhoyj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1bhdm2z</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Marble Jelly</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgytgniwmzoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1bhn97b</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>I don’t own green polish, thank goodness for toppers!</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhn97b</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1bhn1rj</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bhn1rj/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1bidi4x</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>I'm a beginner and this is my first time doing nail art for myself. Love it!</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bidi4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1bi9xlg</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Hot Pink Sweetheart Swirls Stiletto Nails</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0ecfgu8g7pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1bi7l3h</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>@sweetbobanails stan</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dsomf9tcw6pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1bi3lkj</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>3d nail art</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vo4mshac26pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1bi1ef6</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink blocks </t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/13c2z7gzm5pc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1bhypna</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>One of my favorite nail art designs 💅🏼💅🏼</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bhypna</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1bhsrl5</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>new spring nails🌸</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4nbn522x3pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Mar 20 08:07:49 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_24.xlsx
+++ b/data/2024_03_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C427"/>
+  <dimension ref="A1:C569"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7693,6 +7693,2420 @@
         </is>
       </c>
     </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1bj600n</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Pedicure in leg cast</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj600n</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1bj5ydt</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t xml:space="preserve">black never disappoints </t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlu93tqrbfpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1bj10ak</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Looking for XXS press on nails!</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bj10ak/looking_for_xxs_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1bj0qqz</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Would you find a new nail tech?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bj0qqz/would_you_find_a_new_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1bizh24</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Seeking Advice on Peel Off Base Coats and Nail Tips</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bizh24/seeking_advice_on_peel_off_base_coats_and_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1bj3qz6</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Spring vibes</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7v0hqqs9pepc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1bj3c17</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>my nail artist is the bob ross of fingernails</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4xt2zlklepc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1bj3bgn</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>my piggies are so cute 🥹</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q98fwzbflepc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1bj32lu</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Got to be a hand model today</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj32lu</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1bj2v4i</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - A Rogue Haunting</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj2v4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1bj2pe9</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Nearly finished painting my Nifty set from Hazbin Hotel ✨</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gedktm5gepc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1bj2bit</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Just got back into doing my nails! Suggestions?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj2bit</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1bj1vx8</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Don t you love animal print? 😍</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zdel8q569epc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1bj1256</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Easter nails 1 week growth</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/go93z0q92epc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1bj11ev</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Jennifer Y at Russian Manicure NYC</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bj11ev/jennifer_y_at_russian_manicure_nyc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1bj0ukm</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Spring nails 🌷</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjwttxdl0epc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1bj0s6u</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>I couldn’t resist the green🌲🐍☘️</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj0s6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1bj09nk</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Easter Chrome</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wi5x8ygwvdpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1bj03zb</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>I took a recent course, did you like it?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zb13ko0iudpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1biz1zm</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>I think these might be my best nails yet! IN LUUUUV</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rso000mkmdpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1biyy6r</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Bunny nails</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1biyy6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1biyg36</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Yesterday’s set😍 (5 months in)</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2nvf8myhdpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1biy74a</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>could i even get acrylics with nails these short?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cviry554gdpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1bixtu6</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Pop Art Nails (forgive my cuticles)</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bixtu6</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1bixlbj</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Describe this to a nail tech?</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bixlbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1bixke7</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Ready for an Easter egg hunt 🐣</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9i3l63qibdpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1bixff4</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Spring GelX</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7ncx0aiadpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1bixdwt</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>It's almost fishing season</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5uzvq97adpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1bivvfd</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Spring time</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30yovq9mzcpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1bivr50</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>It’s giving neutral mermaid 😍🐚</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bivr50</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1bivqp9</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Need advice on premature wearing.</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bivqp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1bisgfx</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Second set on myself as a beginner nail tech (Flora from Winx Club inspired!)</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bisgfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1biveiz</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pastel lilac nails 💜 Easter Vibes 🐣 </t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dbpsco9wcpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1biv5us</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Coquette</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1biv5us</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1biv29u</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>My nail tech gave me Lisa Frank vibes today 🦄</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdcngq1vtcpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1biuzj0</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Black and gold 🤩</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1biuzj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1biuqfv</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>White ombré 🤍</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9qnit1krcpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1biubro</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Pink and soft glitter</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8chzxfhmocpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1biu43z</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>first time trying polygel with paper forms!</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1biu43z</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1bitvzb</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Spring nails!!</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3jofspflcpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1bitk92</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>A husband on a mission - I really like the design my wife picked for me to do last night.</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bitk92</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1bitk0p</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>once again, my nail tech ate!</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e667xfs2jcpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1biteiv</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1biteiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1bitcox</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Easter Nails 🐇 🐣</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xldzmfnhcpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1bit6zq</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I use a peel-off base under glue-on nails? </t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bit6zq/can_i_use_a_peeloff_base_under_glueon_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1bit1si</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>What nail shape would suit me</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/choqsziffcpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1birie2</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>they like this design</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asg6fa0e4cpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1birasy</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Hello! I know nothing about nails! I got this done yesterday and my girl did a really nice job, but I realized afterwards that I don't like the black tips that I chose, and would like to just have them nude. How hard would that be, would she have to start from scratch?</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xaoow0aw2cpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1bir8ry</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>First time!</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bir8ry</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1biqa5w</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Black flowers</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugqidc8hvbpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1bipsbf</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Found the perfect technique to get this babies welded on 😂</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2iv7u1furbpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1bipqs4</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nail design </t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f70n2p0krbpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1bipb5d</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking to start out </t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bipb5d/looking_to_start_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1bip8kg</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>my first attempt at acrylics! 🩷❤️</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bip8kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1biov0y</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love this nails </t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xla774l7lbpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1biopkz</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Spring colors!</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1biopkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1biofa3</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What to do with these forms? </t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c7ejejt0ibpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1bio8w5</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Why do my nails grow out this shape?</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bio8w5</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1bins8k</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Bunny nails done by my non dominant hand!</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bins8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1bimhvq</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Chillhouse Tips - New Pink Nail Glue is BAAAAD</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bimhvq/chillhouse_tips_new_pink_nail_glue_is_baaaad/</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1bikfe5</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Gore meets Coquette</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jepuoxx9napc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1binabm</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polygel dual forms don’t fit my thumbs </t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1binabm/polygel_dual_forms_dont_fit_my_thumbs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1bin4g0</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Manicure </t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x98js4mo8bpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1bin3li</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Crushed my nail months ago, how can I fix it</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwxs8edi8bpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1bimqs8</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>In love with this new set. Trying for the first time</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5osz4tt5bpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1bim8yb</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Nail growing into my thumb</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w45lkmd02bpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1biljg3</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Tried out some chrome powder for the first time!</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqc2t8vbwapc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1bilauh</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Do these suit me?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irbse0nguapc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1bikcep</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>My spring nails</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rttkeminmapc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1bijaxf</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>in love with this new set my nail tech vin did 🤍</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/umxaxzvrdapc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1bij0d2</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>New mani</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ji0d64zaapc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1bigtwi</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Experimenting with ways to make subtle gradients, any tips? (normal polish not gel)</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jradfsxjn9pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1bifat5</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Ahhh🥹💋❤️</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yd1og6yi39pc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1bj6h1l</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>A Spring Mani feat. Drunk Fairy Polish</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8msf99cvhfpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1bj6203</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Love white polish but....</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bj6203/love_white_polish_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1bj5x3n</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Spring Creme</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3r6fmpacbfpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1bj5al0</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Dyshidrotic eczema after developing an allergy..</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bj5al0/dyshidrotic_eczema_after_developing_an_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1bj59vv</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Toes painted in cast!</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj59vv</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1bj4ti4</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mood Ring Ring Magnet it's like wheel of fortune! </t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z88xwbygzepc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1biyk3j</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Greetings!</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1biyk3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1bj4sgz</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>She keeps swinging and missing</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj4sgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1bj4dx1</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Dupe for Esmalte Glitter Hits 5free in Diamante?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bj4dx1/dupe_for_esmalte_glitter_hits_5free_in_diamante/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1bj346y</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Earth girls are easy (nails in the movie)</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bj346y/earth_girls_are_easy_nails_in_the_movie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1bj2sy6</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - A Rogue Haunting</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj2sy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1bj23gd</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>I can't get over how shimmery this is</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj23gd</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1bj0xkc</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Watermelon and animals</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj0xkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1bj0vfn</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Grerple! (Sirene, ILNP)</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxy9gf3s0epc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1bj0jjz</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Cat monster nails</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wiqouk13ydpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1bj0ghm</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Spring time nails 🌸 the shift is sooo fun</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj0ghm</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1bj02n0</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Reminds me of blue Bic pen ink 🖊</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj02n0</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1bizmuo</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Emotionally unhinged competition...</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9r7vjnyqdpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1bizkun</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Opal nails ✨✨✨</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bizkun</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1bizeoj</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Easter inspired mani</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yn4yc2n8pdpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1biz568</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>I really need some suggestions for a jelly pink polish.</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1biz568/i_really_need_some_suggestions_for_a_jelly_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1biz2zk</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Far from perfect but I'm getting better! Tips and dip powder :)</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7uem1yrmdpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1biylhi</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Brands to try or avoid on Harlow &amp; Co?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1biylhi/brands_to_try_or_avoid_on_harlow_co/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1biyc8c</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Coordinating with my Cotopaxi pack</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ownm30b5hdpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1biy69o</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>St Patrick's Day Shamrock Watermarble</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ovkeuuyfdpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1bivzlh</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Advice needed on reducing premature wear.</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bivzlh</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1bivvuw</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>What’s your fav peely base?</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bivvuw/whats_your_fav_peely_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1bivsh3</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>My nails are a hot mess and I want to fix it...but I'm a little lost on how to :( Halp?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bivsh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1bivpx7</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Esmaltes de Kelly, Smoke</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bivpx7</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1bivn5k</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Spring 💐</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwd63mbzxcpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1biujv9</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Springy jelly skittle</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1biujv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1bitskf</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Queen of Hearts ♥️🖤</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bitskf</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1bitrh7</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Can I make my own blurring base coat?</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bitrh7/can_i_make_my_own_blurring_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1bitjml</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Lumen is offering a refund for Papillon</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlhjyob0jcpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1bisbq8</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Super Shifty 👀</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bisbq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1bis13v</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>St. Paddy’s day clawz 🍀 [OC]</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8384uop48cpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1birn5g</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I've never had cat eye before 🤩💚 I'm in love </t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9ry2tmc5cpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1biqrd8</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Spring Jelly Mani</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1biqrd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1bipz4n</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Iso: Your favorite pastel yellow</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bipz4n/iso_your_favorite_pastel_yellow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1bipvb0</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Wear your protective base coats</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bipvb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1bipuxh</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me find the perfect teal! </t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bipuxh/help_me_find_the_perfect_teal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1bip4ei</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Similar ✨vibes✨ to ILNP Dusk to Dawn?</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqvhjj24nbpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1bio9c7</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>this is my biweekly "thank you" to whoever came up with the U-shaped magnet trick</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bio9c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1bio3kv</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>HELP I want everything</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bio3kv/help_i_want_everything/</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1bio2xd</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>sugar coated shine 💫</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bio2xd</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1binfil</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Cliondah Ghibli update</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1binfil</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1bin7rn</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>These are the nails of a killer, Bella</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bin7rn</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1bin6ty</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Bee’s Knees Lacquer - Love is the Most Powerful Magic</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bin6ty</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1bim1up</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Florals? For spring? Groundbreaking.</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twrgrire0bpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1bilfym</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Shorties &amp; Builder Gel</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bilfym/shorties_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1bikzq3</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Did my nails in honour of favourite pet shrimp, I think he likes them!</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bikzq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1bikyw3</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Applying nail polish to damaged nails?</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bikyw3/applying_nail_polish_to_damaged_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1biktvs</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>ISO: Opal Nail Polish</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1biktvs/iso_opal_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1bik91f</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Tried to dupe Alien Infatuation with my current collection</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7as7sv7wlapc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1bigqd8</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>On the quest of finding the perfect nude</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bigqd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1bj2pzo</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Nearly finished painting Nifty from Hazbin Hotel ✨</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nyf7jvtagepc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1bj1ze9</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Hand drawn on dip with tips in between clients. 45 minutes start to finish</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exxel1j1aepc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1bj1bgj</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj1bgj</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1bj0e0p</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Recent favorite sets 💅🏼</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj0e0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1biypmu</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>New to this, looking for advice</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1biypmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1biyc2k</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Spring nails begin! 🥳</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1biyc2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1biuds2</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Satisfying Top Coat application of broken glass nails!</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vem72c1wocpc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1bitqfb</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Queen of hearts ❤️🖤</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bitqfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1bis3mb</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Freestyled duckies 🦆 🦆</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bis3mb</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1biqz2v</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry nails for spring ~ </t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpbqjysj0cpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1bincsj</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Dollar tree rub on transfers for scrapbooking ftw. Why did no one tell me these work before?!?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtbkrgkfabpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1bimupj</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Painting before attaching gel with fc tips - how to avoid bulk??</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljmd1kdn6bpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1biji7b</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Parallel Universe</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1biji7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1bii76b</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Feeling Blue 💙</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gp8ttcww2apc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Mar 21 08:07:51 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_24.xlsx
+++ b/data/2024_03_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C569"/>
+  <dimension ref="A1:C738"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10107,6 +10107,2879 @@
         </is>
       </c>
     </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1bk0s5t</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>gel x nail by me 🏹</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bk0s5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1bk0lid</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Which nails for a nail-biter?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bk0lid/which_nails_for_a_nailbiter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1bk0egg</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>love this mermaid mani 🧜🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2c2m4hvgxmpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1bjyda3</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>dip vs hard gel??</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bjyda3/dip_vs_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1bjxf7r</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>NEED HELP DESPERATELY</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjxf7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1bjz3et</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Any tips for taking better nails photo?</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6y66hvohmpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1bjytg0</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Rose Quartz 💖</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjytg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1bjwje6</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Advice for protecting/healing nails?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ifi4ml9slpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1bjueli</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI </t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bjueli/opi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1bjqxua</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>can someone give me a guide on how to apply acryllics and make them last?</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bjqxua/can_someone_give_me_a_guide_on_how_to_apply/</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1bjqtx5</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Bloody stumps to handy fingers</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjqtx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1bjlzrc</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Please help with my cuticles and nail shape. Don’t know how to fix weird grown cuticles, help?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjlzrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1bjlhix</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you keep your nails from drying out between painting them? </t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bjlhix/how_do_you_keep_your_nails_from_drying_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1bjvv4y</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>I like this model, it is very cute. What do you think?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvn81rm7mlpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1bjvple</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Thickened polish</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bjvple/thickened_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1bjvkte</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Easter nails</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bjvkte/easter_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1bjvjih</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Spring Butterflies 🦋</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6ionazijlpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1bjvh19</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Love and peace ☮️ and colorful 💜</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/urugedtxilpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1bjvfg5</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NUDE POLISH FOR FAIR SKIN </t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bjvfg5/nude_polish_for_fair_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1bjuohg</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>New set! These are giving Cinderella vibes!</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjuohg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1bjuo1f</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>nail tech eats every time</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjuo1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1bjulxb</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>A Spring Moment</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xg90z78nblpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1bjuhjm</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>removal of acrylic nail + aftercare</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ufa17elalpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1bjud4z</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>classic square french on me by me :)</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjud4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1bjuben</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Holo Taco March Mayhem Mani</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bjuben/holo_taco_march_mayhem_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1bjtouz</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>red themed freestyle ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w434qka04lpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1bjtlw2</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Can you take professional gel polish off at home?</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bjtlw2/can_you_take_professional_gel_polish_off_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1bjtkjx</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>I did my own gel nails!</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjtkjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1bjtgf2</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Fun nail design I did</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjtgf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1bjtclt</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Loving this spring time set 💅</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8dnc7h71lpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1bjt84k</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Good as Marigold 🌼</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4zvbn990lpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1bjssaj</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Gel X Nail Kits / Options Canada (For DIY) - NO APRES</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bjssaj/gel_x_nail_kits_options_canada_for_diy_no_apres/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1bjsn2s</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Question about stamping</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bjsn2s/question_about_stamping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1bjsbld</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Jellybean nails</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjsbld</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1bjs3s3</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>What do y’all think of this set?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0pga41prkpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1bjrnu9</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>baby blue velvet 🩵🫧</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjrnu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1bjrj4y</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Cherry Lemonade vibes 🍋🍒❤️</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjrj4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1bjrg2d</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Commemorating the worst nails my sister ever got done. She paid like $95 for these</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnjjwpplmkpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1bjr27g</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Simple french nails to match my ring! 💍</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ah58k1sjkpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1bjqtpw</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Comparison of colored jelly over silver cateye and just colored cateye?</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/s/2UwFPg6P9T</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1bjqlgq</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Kinda love kinda hate</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjqlgq</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1bjqaws</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Floral Cottagecore</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/slhtr5k4ekpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1bjq64s</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7kvtik5dkpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1bjpm58</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Cherry Blossom Nails! I am obsessed with these, I had to put them on as soon as I made them :)</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjpm58</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1bjouwm</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Want to get into nails again, don't know which method to pick </t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bjouwm/want_to_get_into_nails_again_dont_know_which/</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1bjorbp</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>My birthday nails I did 🤍🦋</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjorbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1bjojy8</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Lollipop set - part 3</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjojy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1bjojjw</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Golden Florals</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zaxh5ttj1kpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1bjo7pg</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>🩷 Painted Polish Blushing Bonbon</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjo7pg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1bjo75a</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Blooming Gel Flowers</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjo75a</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1bjnwtk</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>in love with my glittery nails</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jwe783dqujpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1bjnwi1</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Mourn with me…</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kv4rze5xwjpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1bjnjv1</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Should I wait to put gel extensions on? I’ve been letting my nails grow for a month since over-filing</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjnjv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1bjmsw0</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Have done my own nails for the first time</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjmsw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1bjl666</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Are they cute?</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfk8sttzcjpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1bjl1e8</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Kind of lame but I've never loved my nails more and just had to show them off!</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qs5aghvzbjpc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1bjknfy</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Vampy Red Cateye set I did, are you a fan of spicy or cute nail looks? ♥️ ✧⁺⸜(●˙▾˙●)⸝⁺✧</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjknfy</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1bjkbxj</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Spring Nails💕💐</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rqeu98p6jpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1bjjjwv</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>How do I tell my nail tech that I'm learning to do my own nails?</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bjjjwv/how_do_i_tell_my_nail_tech_that_im_learning_to_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1bjjfgp</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>The BEST Press Ons</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjjfgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1bjjq9f</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Panda &amp; bamboo nails</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qysu8inb2jpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1bjjejo</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Easter egg nails</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjjejo</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1bjixtb</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Chrome French manicure - might be my engagement nails 🤭</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjixtb</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1bjipny</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>My new nails</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2p2fthyuipc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1bjid07</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Pink nail’s 🩷</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wcdhl7fsipc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1bjhda0</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Love finding new ways to use blooming gel</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47jxsvl2lipc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1bjh0uo</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Nails I did</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjh0uo</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1bjavns</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Practicing gel extensions using tips</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjavns</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1bj90d0</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Loving the “pink glow” polishes lately! Growth progress!</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj90d0</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1bjff5v</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fried eggs or flowers 🤔 </t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chnbzv2l6ipc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1bjf9lb</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>My spring nails, done this morning 🌸🌼</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nswjznxd5ipc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1bjet59</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>New set 💅🏼</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxjltg1x1ipc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1bjesm4</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Day 2</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vstddxdr1ipc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1bje3n0</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Finally found someone in my city that does gel nails instead of acrylic!</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bje3n0</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1bjdnn4</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>should I get a new set?</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bjdnn4/should_i_get_a_new_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1bjdjbq</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>🧡</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3v79q6eprhpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1bjd3fp</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>got my nails done !</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97ugslgznhpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1bjd0ql</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>I don't usually use glitter, but I like it, can you vary it a bit or not?</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hd8jlpxbnhpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1bjczqu</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>My favorite set!!🩷</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjczqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1bjcmpr</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Feeling meh about my nails</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0xmqaavjhpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1bjca33</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Blinged out red set❤️</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8o92qcsighpc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1bjc0tg</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Do you think I can make it another week before getting a fillin?</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1od4021ehpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1bjbru0</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to get my gel nails to stop chipping/lift? </t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bjbru0/how_to_get_my_gel_nails_to_stop_chippinglift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1bja8gi</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>This time, my handyman outdid himself</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jto2v3lrugpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1bja33d</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Bunny nails stickers</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bja33d</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1bja26f</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>One-time mani results</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bja26f</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1bj9c1c</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>press on nails</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bj9c1c/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1bk135l</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>New color combo!</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/diih1h2a6npc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1bjyomy</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>She calls it desperation, I call it perseverance</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjyomy</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1bjy9w9</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Frenzy</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmgm42li8mpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1bjxcua</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Chrome flakies</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjxcua</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1bjwxe1</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>It's time for teal</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjwxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1bjwfjz</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Watermelon and animals</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjwfjz</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1bjwci7</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's like painting with liquid steel </t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ag47vqjlqlpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1bjvzng</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Cottagecore</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbvza57fnlpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1bjvc0k</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Swatch, purple palette cleanser</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjvc0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1bjvbkf</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Dany Vianna (original promise), sticker?</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/johc04anhlpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1bjv92e</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>It’s only been 12 hours…the shrinkage is laughable</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzt80qe3hlpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1bjtnil</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Lume Comparisons: Morpho Glow vs Glass Jellyfish ft. La Lune</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjtnil</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1bjtfhz</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Fishscale nails! ♓appy first day of spring to all my Pisces pals.</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjtfhz</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1bjt9e3</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>CG - Good as Marigold 🌼</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xw2evqzi0lpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1bjsfil</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Spring equinox mani ✨</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pct6fyr7ukpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1bjsbia</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Nails are trashed but I have to keep applying polish, what to do?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bjsbia/nails_are_trashed_but_i_have_to_keep_applying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1bjryr7</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Birthday Suit, but French 💕</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjryr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1bjrm99</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>1 coat of Pigeon on Alien Infatuation (middle finger)</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjrm99</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1bjqvzv</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>A broken nail journey</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjqvzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1bjql39</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Can anyone figure out what ESSIE nail color this is??</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjibzag7gkpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1bjqg01</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Unconventional Easter/Spring mani</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjqg01</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1bjq9rj</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Do I Need House of Hades?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjq9rj</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1bjpx0s</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Baby - Phoenix/EDK/Esmaltes da Kelly(received as PR In 2022)</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjpx0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1bjpocp</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Glasswing Pigeon</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjpocp</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1bjp07t</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Chaos skittle</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjp07t</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1bjoulp</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>I love, LOVE glow-in-the-dark polish!!</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjoulp</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1bjo9ox</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>the shimmer is real! 🌈💎</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjo9ox</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1bjo6xo</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>🩷 Painted Polish Blushing Bonbon</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjo6xo</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1bjo3fs</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Another Dust to Dust beaut</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4tc1xpbyjpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1bjnuzh</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>How can I make this polish more flattering for my skintone?</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjnuzh</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1bjnn3p</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>My polish barely lasts a day. What am I doing wrong? :(</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bjnn3p/my_polish_barely_lasts_a_day_what_am_i_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1bjng78</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Round 2</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwtg60eltjpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1bjnfv1</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Serpent Venom and Kraken’s Wrath - Cuticula</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjnfv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1bjn7ge</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>My first go at a flakie gradient!</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fce3lujtrjpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1bjmxq7</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>New Holo Taco Collection, thoughts?</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjmxq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1bjmb43</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>What affordable websites in Canada are there for nail polish?</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bjmb43/what_affordable_websites_in_canada_are_there_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1bjlm0m</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Shifty Shades of Grey</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/j18jSZy</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1bjl8hd</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Looking for a creme polish as close to this color as possible</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ok15cbghdjpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1bjjldz</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>ILNP Rosewater super gritty</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjjldz</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1bjjd6m</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Ready for Spring</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30hsn1rnzipc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1bjiwkd</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Nail polish refuses to stay on my nails</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjiwkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1bjhkn4</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Lumen Glass Jellyfish &amp; Snow Shadow</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjhkn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1bjhh69</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>🐝🍯Winnie the Pooh🍯🐝</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjhh69</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1bjgm7j</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>History of Coronation. Last few bottles of its, "last drop," available tomorrow, 3\21.</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eonx2jkifipc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1bjftuu</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Essie gel setter changed my polish colour?</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqwxog8n9ipc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1bjfp5c</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Green and Blue skittle</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjfp5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1bjfl16</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>This is so neurotic of me, but does anyone recall what time of day Cirque dropped Coronation last time it came around?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bjfl16/this_is_so_neurotic_of_me_but_does_anyone_recall/</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1bjanz6</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Do you need to put base coat on press on nails?</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bjanz6/do_you_need_to_put_base_coat_on_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1bjbcy3</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Brand new gel overlay is peeling????</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bjbcy3/brand_new_gel_overlay_is_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1bja873</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Green with a subtle shift</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bja873</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1bjcn2u</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>🧚🏼‍♀️✨ Polishes Used: ILNP (Shade: Fairy Dust) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjcn2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1bjcp8g</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>🌤️🩵 Polishes Used: ILNP (Shade: Up Above) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjcp8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1bjehdw</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Line work practice success!</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/le60wkrczhpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1bjdy75</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Beach nails!</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhacrph4vhpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1bjdt32</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>I took a crack at Opal Nails</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psttgb3hqhpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1bj9slc</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>New manicure! I'm obsessedddd 💚</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pefsxiwipgpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1bj8wjt</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Loving this simple look lately and current growth.</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bj8wjt</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1bk0s4e</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>my handyman got me in the mood</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gniicd3a2npc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1bjxibu</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Abalone shell inspired</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjxibu</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1bjws83</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Obsessed ✨✨✨</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjws83</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1bjvrn9</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Dude press-ons!</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qilov4rhllpc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1bjvqcw</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Stitch!</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/shi2hsb6llpc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1bjv6zt</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Cute as heck</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwsll67lglpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1bjv5xq</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Doing a french nails with chrome powder.</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/in8tebppflpc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1bjuk5j</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Practicing different techniques</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5adkjm58blpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1bjtxao</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>i think i found one of the most cursed nail pic poses</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjtxao</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1bjtm7l</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Frog recreation set</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8nstfee3lpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1bjsotm</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>How are you doing intricate nail designs on your own nails?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30zhvoc6wkpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1bjq41e</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Inspiration on left and result on the right. What do you think?</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sg6fn12qckpc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1bjom3g</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Lollipop set - part 3</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjom3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1bjoixm</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Golden Spring</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edngjdtf1kpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1bjobt5</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Obsessed 🔥</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bnen93tzzjpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1bjmz1f</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💙🐆💙🐆💙 reminds me of Lisa Frank </t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fofdom83qjpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1bjll5l</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Re-making my first nailart!</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjll5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1bjkufe</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Cherry Blossom nail art</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjkufe</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1bjjrw4</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Panda &amp; bamboo nails</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gbbz2en2jpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1bjj559</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chasing rainbows 🌈 </t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehwsc0i1yipc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1bjictl</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Miraculous Ladybug and Cat Noir Nails</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ubp128odsipc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1bjhpq7</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Did my friends nails with Pink Panther decals she found at vintage store</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjhpq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1bjhmcx</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>the coolest nails I have ever had!</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjhmcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1bjhi1v</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Nails I did</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bjhi1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1bjfmm5</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Not weird, just limited edition</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nj14giv48ipc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Mar 22 08:08:27 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_24.xlsx
+++ b/data/2024_03_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C738"/>
+  <dimension ref="A1:C870"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12980,6 +12980,2250 @@
         </is>
       </c>
     </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1bktfu0</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Fresh nails 🥰</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krkvv2gy6upc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1bkszzd</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>what am i doing wrong!? (builder gel edition)</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bkszzd/what_am_i_doing_wrong_builder_gel_edition/</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1bkstf6</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Red Cet eye ombre!</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkstf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1bkrzk4</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Easter nails for my daughter :)</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkrzk4</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1bkrm6e</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Nails suddenly weak and breaking?</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bkrm6e/nails_suddenly_weak_and_breaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1bkpwqx</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Anything is possible.</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkpwqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1bkp9tj</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Weak and sensitive nails. What are my options?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bkp9tj/weak_and_sensitive_nails_what_are_my_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1bkns5n</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Does anyone know the difference between Korean gel vs western gel polish?</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bkns5n/does_anyone_know_the_difference_between_korean/</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1bkkm2p</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Spring nails 🌷</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkkm2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1bkk8r3</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>When you can't decide which color to wear...</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkk8r3</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1bkgepm</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Nail noob</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8uypzd1sxqpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1bkcjfh</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>How do you grow ur nails thick and strong</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bkcjfh/how_do_you_grow_ur_nails_thick_and_strong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1bkeu7m</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Products that help with damage from Gel-X? Help??</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkeu7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1bkenu0</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Russian/dry gel manicure recommendations near Hackensack, NJ</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bkenu0/russiandry_gel_manicure_recommendations_near/</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1bkdvp9</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Hand painted nail art on natural nails</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkdvp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1bkdn75</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Can I apply a layer of clear gel polish over my press on nails?</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bkdn75/can_i_apply_a_layer_of_clear_gel_polish_over_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1bk4uou</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Help! Natural nails</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jlxvuyxyfopc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1bk2oji</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Spring Nails Inspo by Hannahtaylor</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fef6uay0rnpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1bkquhl</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>One of my most recent works, what do you think?</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6s2p9rubtpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1bkqhxv</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Mermaid vibes 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/01kck2sb8tpc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1bkpqu1</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice </t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bkpqu1/advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1bkpnlt</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Never did short squares on my natural nails before, I kinda like them </t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3qx28d40tpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1bkpgtz</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>I love fun designs</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lapx0ltayspc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1bkp0vz</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bkp0vz/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1bkoa9y</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Nail sets I’ve done recently! Hard gel structured manicures on my clients’ natural nails</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkoa9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1bko2v5</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Question about builder gel</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bko2v5/question_about_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1bko2dy</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Gel X and Soft Nails</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bko2dy/gel_x_and_soft_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1bknsy3</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>oh no now I might always have to have textured nails</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/099tl0ccjspc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1bknlgj</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Constructive criticism please</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bknlgj</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1bknfa3</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Simple pink frenchies i did🩷🩷💖</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfe1yrqzfspc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1bkmqck</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Badger badger mushroom mushroom</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xracek9x9spc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1bkm7bc</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>BANANA 🍌</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcawtl7h5spc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1bkm0bj</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Easter nails!</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkm0bj</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1bklhv2</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Can cuticle oil make my fills not last as long?</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bklhv2/can_cuticle_oil_make_my_fills_not_last_as_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1bklgbz</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>🌈 nails</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxxrly4dzrpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1bkkcmb</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Fresh Set!</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6aobwq3lqrpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1bkjwes</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Holographic flames🔥</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qo6l0m6nrpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1bkjhb4</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>i'm in love! &lt;3</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkjhb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1bkjc0c</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Coffee French mani</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tp28jua0jrpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1bkihsl</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Love love love</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pvhx5syrcrpc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1bki4ux</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>First attempt at rainbow smoke nails 🌈 💅🏻</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2twl0rbarpc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1bki28i</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>my first time getting a style like this</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4eq72mgt9rpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1bki22x</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Magnet recommendations?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bki22x/magnet_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1bkhpkb</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>🐝 🌺</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s715zvp97rpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1bkgx8l</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail drill charger </t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gplw4xj1rpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1bkgh0w</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>I never get fake nails but I did get tips and dip spent 60$. Total bill 95. One came off in 10 days. 2 more popped off 2-3 days later. Would you ask to get them fixed at the salon you went to.</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bkgh0w/i_never_get_fake_nails_but_i_did_get_tips_and_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1bkfk00</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Has anyone tried this brand before? If so, how is it? What’s your favorite/least favorite product?</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gyd56r3jrqpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1bkfexv</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>The gloss is glossin’ on this one!</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dkmmpthqqpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1bket1d</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>I paid $200 before tip for my mom and myself. Is this normal?</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bket1d/i_paid_200_before_tip_for_my_mom_and_myself_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1bke18i</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>What can I do to avoid hurting my nails?</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wisw7sfgqpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1bkdtlw</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>my nail tech quit and i didn’t find out until i arrived for my appointment. wanted to leave right then but instead had someone else within the salon do them. not sure if i should laugh or cry. i hate everything about them.</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkdtlw</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1bkdr5b</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Like stars ⭐ in the sky </t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q85qksnceqpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1bkc8vo</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Bit my nails for 15+ years, recovered from it 🎉</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkc8vo</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1bkc2ir</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Stardew themed nails 🌱</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkc2ir</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1bkbu6e</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Textured Birthday Nails💅🧁🖤🎉</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkbu6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1bkbf27</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Looking to buy press-ons to paint and sell, any recos for good blanks?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bkbf27/looking_to_buy_pressons_to_paint_and_sell_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1bkb1jc</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Girly but edgy cherry nails</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkb1jc</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1bkakq7</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Got a gel nail kit for my birthday - here is my first attempt at designs!</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5vfq5ecrppc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1bkacwt</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>I did my Polygel Nails with cat eye effect (the first time) and I'm a little proud of myself 🙈</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkacwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1bk7v9a</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Been having luck keeping them long for my next mani</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbd19g9v6ppc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1bk7ryb</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Question for any nail techs?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bk7ryb/question_for_any_nail_techs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1bk7j37</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Trying to avoid cutting my nails before a manicure… help?</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/koibbxp64ppc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1bk78ct</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>My first at home gel Mani!</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rkn9npsp1ppc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1bk714m</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Royalty nails</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6ya9l720ppc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1bk6av8</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Blooming 🌸</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwej0m4utopc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1bk5hy8</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Magenta for a girls’ trip!</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwqehp1emopc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1bk551t</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first time press ons </t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ktq3ydviopc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1bk407b</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Shooting Star 🌠</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bk407b</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1bk3uqi</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Press &amp; Go Nails at the beach</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bk3uqi/press_go_nails_at_the_beach/</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1bk3cch</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Nail polish always destroys my nail health:(</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6j8xblmdznpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1bk2y8g</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Has anyone tried the beetles pre-etched nails?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ig3415younpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1bk2ald</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Spring Colours</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3bn9pg6mnpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1bk23q5</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>My very first full hard gel built (no tip) made set (untrained)</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bk23q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1bk2041</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>would you run and fill these??</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xnqol9dinpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1bk1xrz</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Nail broke like this yesterday. Is it okay to make a new poly gel nail, or should I let it grow out a bit?</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znrcqlwnhnpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1bksir7</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Paint it Pretty Polish - We're not in Kansas anymore</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bksir7</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1bkrcct</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>fly high soldier 🫡</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkrcct</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1bkqzqf</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>My friend recently turned me on to Emily de Molly, and I discovered thermal polish. I think I'm officially addicted.</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkqzqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1bkqn1o</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>ILNP Clover - thank goodness for the sparkles.</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bkqn1o/ilnp_clover_thank_goodness_for_the_sparkles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1bkq5h7</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupe Request </t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bkq5h7/dupe_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1bkpfbw</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Favorite Set</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkpfbw</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1bkp06l</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jello jello and nail glue </t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bkp06l/jello_jello_and_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1bkobcy</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Vessie de Mer</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkobcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1bko53q</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Nail Healing Journey</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bko53q/nail_healing_journey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1bknx5v</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Experiences with Fany Gloss sheers/jellies?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bknx5v/experiences_with_fany_gloss_sheersjellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1bkmsid</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Thermal crackle</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkmsid</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1bklse5</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Questions about pushing back my cuticles</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bklse5/questions_about_pushing_back_my_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1bkljks</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Multichrome flaky</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkljks</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1bkkuys</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>BKL Choose Life &amp; Queen of the Valbaran Fae</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkkuys</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1bkknzn</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>What are our thoughts?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkknzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1bkk97q</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Science question! (not great picture for tax)—Has anyone tried to make your own blurring peely base?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pq1293ovprpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1bkk00l</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Cirque *Lagoon* Jelly</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkk00l</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1bkj8om</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Your tips, but better</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pu2xkeyairpc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1bkj8h2</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>When does the Polished Gamers Box happen?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bkj8h2/when_does_the_polished_gamers_box_happen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1bkicug</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>🩱👾🔱</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkicug</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1bki134</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Some Spring Nails</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bki134</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1bki0s5</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Juicy</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bki0s5/juicy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1bkhtht</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Is it h-urb or urb?</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pybi4hj18rpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1bkh0zs</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>glowy skittle</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkh0zs</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1bkfnas</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Earthy vibes</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jj3ex207sqpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1bkfflh</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Wild Nude (114) Essie with matte top coat</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jlth5hnqqpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1bkf0dn</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>If you have sensory issues with files, try a glass file</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o03xmiginqpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1bkesv4</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holo, My Beloved </t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kegvkqwzlqpc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1bkd8rf</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Swatched my recent Lumen purchases… 🧐</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkd8rf</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1bkcbds</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>smokey sunset</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkcbds</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1bkbf7t</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Blue cross cuticle remover</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bkbf7t/blue_cross_cuticle_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1bkaswi</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Glass Ceiling + Jade Jelly</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkaswi</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1bkahaw</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Moon 🌙 River</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkahaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1bk92dc</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Spring holo (even though the weather is not very spring like)</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptttz0gyfppc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1bk8c09</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Update: How can I make this polish more flattering for my skintone?</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bk8c09</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1bk80fh</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Help repairing damage</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bk80fh/help_repairing_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1bk7y4d</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Pour one out for me</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bk7y4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1bk71kp</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Thermal beauty: Eb &amp; Flow</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bk71kp</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1bk42ny</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Shooting Star 🌠</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bk42ny</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1bksrc9</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>No name but it looks great!</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bksrc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1bkr5vu</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Want to start doing my own nails but don’t know where to start. Help please! (Not my pics)</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkr5vu</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1bkmgue</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>An ode to Spring</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fk9inwwo7spc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1bkmggz</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Puppy pawty 🐶💕🎉</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ale35zl7spc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1bkmanw</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>BANANA 🍌</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0w54io86spc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1bkkq8h</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Spring nails 🌷</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkkq8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1bkhgem</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Froggy nails! (I'm a beginner)</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c87lseqd5rpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1bkdpzy</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Spring dreams!🦋⛓️🎀💅🏽🌊</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4kxx6bp2eqpc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1bkd7qz</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Blue China nails</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3516fpgaqpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1bkaooj</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Dotting flowers is a lot harder than I expected 😩😅🌼</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hf1fqwc6sppc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1bkanjb</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>First time trying nail designs - Would love to know what you all think!</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5impqyhxrppc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1bkag3g</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Part 3</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkag3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1bkaby7</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Part 2.</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkaby7</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1bka9if</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Sets I’ve made lately</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bka9if</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1bk8oai</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>I'm not a professional, but I like to do my nails</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4z0fsp61dppc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1bk6dmh</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Tried some cloud painting ☁️</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bk6dmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1bk63s6</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>I love my lava lamp nails</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwa719u3sopc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1bk5m96</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>I was bored..</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jqqn84lnopc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Mar 23 08:06:53 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_24.xlsx
+++ b/data/2024_03_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C870"/>
+  <dimension ref="A1:C1022"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15224,6 +15224,2590 @@
         </is>
       </c>
     </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1bll69l</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>After years of doing only brown or nude square nails</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fz3ka2ktx0qc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1bll5wr</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>my nail tech got that skills</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rbkvxzkgx0qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1bll5cn</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Gems</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bll5cn</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1blk0b3</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Paired these lil Gudetama decals with an orange chrome🍊 my favourite is the toast🍳🍞</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blk0b3</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1bljtst</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>3rd set with builder gel. How’d I do?</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bljtst</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1bljeo1</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Q for the Nail Techs - Amazon gels?</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bljeo1/q_for_the_nail_techs_amazon_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1blixy7</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>My new set of nails</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blixy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1blimhp</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>I’m back again! This time with a crazy 3D Easter nail set!</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blimhp</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1blexy6</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Omg can this be salvaged??😭</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blexy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1bli9dc</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Nails I created with hard gel!</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zu9wgy4040qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1bli4qc</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Stunner</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bli4qc</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1blhg32</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Nail care after acrylics</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9zqh1elwzpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1blh51w</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>How to fix a broken nail.</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blh51w</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1blg5tz</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>I’m struggling to figure out what the best color(s) to paint my toes for Easter.</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blg5tz</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1blf6fk</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic short almonds </t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3eu36q7xczpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1blexuc</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Fairy Godmother from Double Dipp’d (chromed over itself on middle &amp; ring)</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blexuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1blerys</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do nail techs prefer for me to not watch them work? </t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1blerys/do_nail_techs_prefer_for_me_to_not_watch_them_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1bler7x</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Birthday nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mviv2opg9zpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1blepq8</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Flowers and pastels are a must for spring right?</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blepq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1blencv</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did Essie reformulate their base coat? </t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1blencv/did_essie_reformulate_their_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1blegk2</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Tried out the butterfly nail trend and i LOVE</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jjhqetw47zpc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1blec7l</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>My Recommendations for salon-quality nails at home!</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blec7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1ble06k</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Is Oxxi brand made in USA or in China?</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ble06k/is_oxxi_brand_made_in_usa_or_in_china/</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1bldxr2</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Easter egg candy</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2tqfafyy2zpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1bldv9z</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>What style do you prefer?</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxu0y9cf2zpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1bldt9u</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Blessed Spring!</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/643s2ywy1zpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1bldprw</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Would I be the asshole to go back to my nail salon and complain/ ask for a redo?</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7byplv71zpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1bld36l</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>thank you TikTok shop 🫡</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9aw7kk8gwypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1blcpbo</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Something similar to Henna?</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1blcpbo/something_similar_to_henna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1blc1uz</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Loving my spring nails💜</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1g4mbvioypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1blbwzx</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Butterfly nails❤️</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrnbw9dmnypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1blbw0o</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love this color so much </t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sn4nafuenypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1bl4p74</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>New set made by me on me</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl4p74</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1blarj7</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Fave 💅 💕</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2m3qd7p1fypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1blajew</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t xml:space="preserve">got my nails done yesterday at my fav place </t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhrbmvcddypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1blacrx</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>I love the glitter. 😍</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccq30nnzbypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1bla9ew</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Nails nails nails</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7kfg2babypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1bla8ca</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5rxns03bypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1bla69j</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Anyone know where I can buy just the foam insert part?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bla69j/anyone_know_where_i_can_buy_just_the_foam_insert/</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1bl9ykp</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Trying to manifest spring 🌿</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl9ykp</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1bl9eyz</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Butterfly 🦋</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl9eyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1bl9e7d</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>So close to Easter m&amp;m colors...</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b025gw8r4ypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1bl8vx1</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Applied a new set of press-ons and the glazed effect got ruined after I attempted to file them down</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lm6h5m501ypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1bl76tf</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>I love bright colors, especially red just drives me crazy</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvnf59egoxpc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1bl6yfu</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Strawberry fields 🍓</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/riui148xmxpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1bl6nto</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>🖤🖤</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lfpo7tbrkxpc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1bl6nnl</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Tragedy struck today 😭</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fhbat2qkxpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1bl66sz</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Anyone else’s state not receive their spring memo yet?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsi9e5pahxpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1bl5n6x</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>🐝 Bees &amp; Hydrangeas 🪻</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f99fynb9dxpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1bl55cr</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>From a Deborah Lippman email - so pretty!</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2oadu92b9xpc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1bl4z3h</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Diamond are a girl best friend </t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gz2sog98xpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1bl4m5d</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>My dominant hand has shorter nails than the other</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl4m5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1bl45i1</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>How do I keep my cuticles from looking like this</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1h9s2tqb2xpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1bl3qqu</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Guy looking for manicure advice</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bl3qqu/guy_looking_for_manicure_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1bl3at5</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Frosty Nails</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl3at5</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1bl2kdj</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Metallic lines! 🤍</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rw40e88mqwpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1bl2imm</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Please rate this out of 10</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkpmxdv8qwpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1bl23pe</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Spring nails 🌸🌼 Inspo from @stylebyreags on TikTok!</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl23pe</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1bl1s9b</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Chipped nails</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bl1s9b/chipped_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1bl10j3</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Spring Inspo</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g08avoatewpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1bl0xw1</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Someone’s nails inspired me! Credit to u/cosmiccmermaid !</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl0xw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1bl0pt3</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>The inspo pic I shared with the nail tech was a bit more refined than what I got…🥲</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl0pt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1bkyje2</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Not sure if my salon has ridge filler; what are some design choices to mask them if not?</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7y5kt0tnuvpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1bkrhqy</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Questions from a newbie</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bkrhqy/questions_from_a_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1bl1p51</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>OPI one chic chick with chrome 💛</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/va3dm8w1kwpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1bl170y</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>First time taking off BIAB from my natural nails</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl170y</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1bl0jnm</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>21st Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl0jnm</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1bl0h17</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>At least the nails are in Spring mode</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00y6wbalawpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1bl0ee2</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>DIY nails with gel x and ohora</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl0ee2</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1bl07ek</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>I usually do Gel-X nails, decided to give BTArtbox a try for a quick new set. OBSESSED with these🤎</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxjwmtxj8wpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1bl04io</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Help! Newbie Color Issues</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl04io</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1bkyz5y</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Pretty plain and simple but I love them!</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkyz5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1bkywzr</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Girly flames 🔥</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzeoi77yxvpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1bkxkxf</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>St. Patty's before it's gone</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmbxsxjclvpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1bkx8ch</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>learning how to do my own nails</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfg73vothvpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1bkx0mf</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>I want to become a nail tech but don't know the first thing about nails!</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bkx0mf/i_want_to_become_a_nail_tech_but_dont_know_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1bkwt8z</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Milky</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkwt8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1bkv88t</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>New pink leopard nails</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkv88t</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1bkunl4</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Best affordable gels?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bkunl4/best_affordable_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1bkudfh</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Three months later and still one of my favorite sets i’ve had</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkudfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1bllufb</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Akzentz and Light Elegance</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bllufb/akzentz_and_light_elegance/</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1blkd8k</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>OPI samurai breaks a nail with added glitter !</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blkd8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1blivvq</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>What’s the perfect turquoise?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1blivvq/whats_the_perfect_turquoise/</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1blifph</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Does anyone know why my nails are curving like this?</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blifph</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1blie3x</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>so glowy 🤩</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l1f445s650qc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1bli5po</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>ILNP - Shooting Star</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qd5gkeq030qc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1blhw13</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Monarch Nails</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blhw13</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1blhrsw</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Once Upon a Time- Vanessa Molina</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blhrsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1blhq0y</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Builder gel in a bottle?</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1blhq0y/builder_gel_in_a_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1blh958</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cuticula did not disappoint </t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/621p0nqxuzpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1blh6fp</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Weekend sparkles</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blh6fp</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1blgwzz</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Shimmering strawberry milk goodness 🐄🎀✨</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blgwzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1blgtcy</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! Need magnet advice! </t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1blgtcy/help_need_magnet_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1blgj3z</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quick drying options? </t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1blgj3z/quick_drying_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1blf4ad</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Fourth time painting my nails improvements</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blf4ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1bleyrh</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Help! Can someone explain this weird discoloring?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bleyrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1bleq24</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Pictures of my nails in the car &gt; pictures of my nails literally anywhere else</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k98555f79zpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1blemnm</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>First attempt at poly gel. Give it to me straight…do they suck?</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blemnm</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1bldj79</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Help me choose my "first week at new job" polish?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bldj79/help_me_choose_my_first_week_at_new_job_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1blcypr</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Emily de Molly Under the Surface</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2mtgb6ivypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1blcfkt</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What colour polish in your collection works for most occasions, events, or themes, and why is it purple? </t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1blcfkt/what_colour_polish_in_your_collection_works_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1blbdql</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Purple and Green 😍</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulw3oo3ojypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1blbby4</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Been staring at my nails all day</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/olgq57s6jypc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1blb8of</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>I am ridiculously sad that I can't do certain designs</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tjrd06cliypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1blb63i</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Favorite local nail polish</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvxer7a2iypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1blb5pe</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Obligatory spring florals</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blb5pe</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1blap0i</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Essie's Tropic Low is stunning</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blap0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1blaohf</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>I LOVE Thermals!!</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blaohf</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1blabec</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>My take on the Magic Mirror Mani</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blabec</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1bla8wy</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Anyone else do their nails during Zoom meetings?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dgyxgtw6bypc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1bla02h</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Oceanic Easter pastels 🌊🐣</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bla02h</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1bl9t8u</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Skittle mani ft Cirque Colours</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl9t8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1bl9cwp</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Creamsicle Dream</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl9cwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1bl784l</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Essie Odd Squad</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84lh5xitoxpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1bl7805</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Nails Inc - That Euphoria Life</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ov4a6bbtoxpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1bl70wm</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Pop-ing into spring</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mpvrgiwcnxpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1bl6mxx</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Found a loose piece of topper glitter so put it on the accent nail!</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l90zo2kjkxpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1bl6l5j</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Picture Polish's Blossom - "Fixing" a disappointing polish</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl6l5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1bl637v</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>essie base coat rough on nails?</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bl637v/essie_base_coat_rough_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1bl5bfe</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>ILNP Neutrals for days</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qay8e1buaxpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1bl4v95</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Native American Owned Indie Polishes?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bl4v95/native_american_owned_indie_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1bl4hxv</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Pink Suede, BAE, Sand Viper, and Sweet Pea Comparison</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl4hxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1bl47jj</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>It’s Just A Phase</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79eltokp2xpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1bl3kr9</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Rosary Pea plus some comparisons</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl3kr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1bl24ku</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Wasn’t feeling good so made myself feel better with my favourite colour</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vt5k7qpanwpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1bl1dix</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>It’s springtime!!</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uho8447khwpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1bl14f1</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>What's your One That Got Away?</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bl14f1/whats_your_one_that_got_away/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1bl12zt</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>"Blushing Apricot" Using Drunk Fairy Polish</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f06kue5cfwpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1bl0xi4</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>DVN in 3 different lights</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl0xi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1bl0x6z</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Slowly getting better at applying magnetics</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl0x6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1bl0uq6</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>I'm still not over winter colors❄️</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl0uq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1bl0jh0</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>New LynB collection</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl0jh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1bl0erg</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>I love the color combo but, I didn't realize it was a crelly for the yellow. Thoughts on mixing finishes?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl0erg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1bkzf0p</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>dookie nails</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3r42ozh82wpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1bkzeje</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>So obsessed with Poison Garden by envy lacquers that I just have to show it off in different lightings</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkzeje</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1bkyt09</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Dip on just my thumbs?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bkyt09/dip_on_just_my_thumbs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1bkvp2f</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>OPI XPress/On in Editor in Chic… Never tried glue-ons but these are absolutely stunning!!!</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kzx4ozo0vpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1bkvozu</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>WAAAAAHHHHHHHH</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcs6xg9o0vpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1bkvawd</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Pink leopard nails 💕</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkvawd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1bkuxt1</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jelly gradient </t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v72hqv35rupc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1bllq05</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Junk nails I’ve done recently :)</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bllq05</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1blhmsx</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Easter nails!</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blhmsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1blf7zi</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>What vibes do these nails give? ✨ done by me.</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6ibcpladzpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1blefw3</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Freehand painted nail art by me, sculpted from acrylic</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4t2eiqp6zpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1bl8taq</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>snooki vibez</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl8taq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1bl67dy</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Anyone else’s state not receive their spring memo yet?</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ug480uwehxpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1bl5mhz</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Just did my nails!🌸</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bl5mhz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1bl3os9</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mis uñas </t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bij1814wywpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1bl363a</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just got some gel polishes to play with for the first time, and my son tole me I should do and Easter set (I've been making my own press ones). Polka dots and bunnies are done in acrylic paint, matte top coat </t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fzz8a23vwpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1bkz274</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Spring Inspo</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgvakk08zvpc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1bkxabq</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>New manicure 🐆💕</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkxabq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1bkx23v</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Purple flames, purple flames 🎶 💜</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bkx23v</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Mar 24 08:07:11 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_24.xlsx
+++ b/data/2024_03_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1022"/>
+  <dimension ref="A1:C1187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17808,6 +17808,2811 @@
         </is>
       </c>
     </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1bmfaq7</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Thoughts in these onez? My friends are unsure if they like the middle finger so its making me iffy? I tried the blooming gel for my first time on the middle fingers</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bmfaq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1bmf6o2</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>My chrome pink nails 🩷</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bmf6o2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1bmelfr</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Most people do pastels for spring, I’m more of a neon girl 🤦🏾‍♀️😂</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0oqao421d8qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1bmdvrf</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>In need of nail growth tips ASAP!!</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bmdvrf/in_need_of_nail_growth_tips_asap/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1bmdob6</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>French-ing 🥰 I really like how the decoration turned out 😌</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23gg24w028qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1bmcwrc</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set for next three weeks :) </t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1q0r2mf4t7qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1bmchux</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Just tried press on nails yesterday for the first time and there is moisture underneath.</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bmchux/just_tried_press_on_nails_yesterday_for_the_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1bmce1e</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81favpvin7qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1bmc34r</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Idk, i badly need some creative ideas. Help a girly out, thank you 😭❤️</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1fd4yfik7qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1bmbz9e</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Essie Pearly White 🤍</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1j7oh9ej7qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1bmbrn7</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>My nail tech is magic</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bmbrn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1bmalz4</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Spring nails! I'm in love</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a96ialx767qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1bmaerj</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>PSA: Don't be an Idiot Like Me</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zldo7fc47qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1bma92e</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Does anyone else have different shape preferences for different fingers?</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bma92e/does_anyone_else_have_different_shape_preferences/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1bma4si</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>What Do You Think About My Easter Nail Set?</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rkg56ypp17qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1bm9vhq</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>My friend is so amazing at nail art🐚🌿</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm9vhq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1bm92ka</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>I only started painting my nails a few months ago, any tips?</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijkqr734s6qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1bm5vrp</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>How to ask nail tech how much they would charge</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bm5vrp/how_to_ask_nail_tech_how_much_they_would_charge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1bm0ywc</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Be honest; did I get ripped off?</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm0ywc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1blyqlz</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jaj6x0ak4qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1bm8ryz</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Classic French with Modern twist </t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6ct2zujp6qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1bm8jgk</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>She went off ✨</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cew40elfn6qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1bm8hz5</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>My favorite color 🩵</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7vt29tym6qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1bm8axl</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>April nails</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm8axl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1bm869t</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Loving these!</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm869t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1bm7vq4</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>What do you think about my new set 💀</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0ncri1uh6qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1bm7cge</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>I told myself that they weren’t that bad…</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm7cge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1bm6wt3</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Suggestions on what to do with my nails. Recovering nail biter and want something cute but not sure what to even ask for</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm6wt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1bm6pyg</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are the best nails to put on my own nails that I bite to prevent me from doing it? </t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bm6pyg/what_are_the_best_nails_to_put_on_my_own_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1bm6gh4</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Loving this shade of green</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmroc6ia66qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1bm61do</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>🤔</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bm61do/_/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1bm5dod</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>I loveeee these 🌸💕</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mk5rvqgwx5qc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1bm593l</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Too thick?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm593l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1bm4nsc</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>First time doing gel x, any advice?</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm4nsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1bm4g0j</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>New nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gw1ymi5nq5qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1bm4f1x</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Bling bling 💅🏻✨</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm4f1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1bm4bnw</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Happy Easter!</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm4bnw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1bm45us</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Got Dip Nails for the 1st time</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uaojqz3jo5qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1bm409t</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t xml:space="preserve">spring details </t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ttz9w3tcn5qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1bm3qda</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>RUN TO DOLLAR TREE Y'ALL</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ma5yldg6l5qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1bm2xpi</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwtxo339f5qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1bm2o3z</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Nail shape is important</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm2o3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1bm2kqm</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>DIY lavender tips ft Virginia blue bells 🌤️</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm2kqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1bm2f4k</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>One of my favorite sets ever😍💙🩵</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ld0ez7nfb5qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1bm1urd</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Surgery in 3 weeks, so time to go back to my own nails….</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm1urd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1bm1sny</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Ready for spring!</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm1sny</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1bm1s8i</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice </t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bm1s8i/advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1bm1g71</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should you give your nails a break from dip? </t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bm1g71/should_you_give_your_nails_a_break_from_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1bm1ae6</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Back to shorties 🩷💚</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm1ae6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1bm13od</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>New Set!</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8l37swcq15qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1bm0w29</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>About 9 months into doing my own nails. I think I’m finally getting it!</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6utr4h605qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1bm0vd0</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Fresh springy set💅🏼</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/giaq2ke105qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1bm0btl</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>What do you think about my work? 💙💗💛</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm0btl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1blzn34</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Looking for nail lamp recommendations</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1blzn34/looking_for_nail_lamp_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1blz89p</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Full cover tips for short nail beds. Apex always ends up near my tip</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xw5r205yn4qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1blyda8</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Help with prep</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybflpqsjh4qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1blxydy</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>So proud</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blxydy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1blxnr4</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Manifesting a sunny Spring 🌼</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blxnr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1blxmgt</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/131agbqxb4qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1blxgl3</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First gel set I've done myself, one week later 😅 </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8v91wjpa4qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1blwm7m</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what products should i buy for beginner gel nail </t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1blwm7m/what_products_should_i_buy_for_beginner_gel_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1blwj5l</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Strengthening natural nails </t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1blwj5l/strengthening_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1blwa9l</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Made my first press on set !</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ly8yazjs14qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1blw3wm</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>UV gel safety</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1blw3wm/uv_gel_safety/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1blvn1j</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Feeling like a fairy in a whimsical garden with my new nails 🧚‍♀️🍄</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flexkxlyw3qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1blpbd5</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>What's the purpose of prepping nail bed and pushing back cuticles</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1blpbd5/whats_the_purpose_of_prepping_nail_bed_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1blus1c</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Speckles</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhhy8lzhq3qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1bllatl</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Idk how to get rid of the wwird leather texture </t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5impzb8z0qc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1blkjw7</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Why does this always happen when I get my nails done ?</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blkjw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1blk4li</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>I’m so self-conscious of my hands. I have to keep my nails short because I wear contacts. Can someone point me in the right direction for the shape?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blk4li</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1bltzrh</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>New nail day :) I'm obsessed</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ezyy253k3qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1bltuwu</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Eccentric Empress</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bltuwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1bltp9x</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Chrome thick french tip 🤍✨️☁️</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0uicr22i3qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1blt430</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Hooked Nails</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1blt430/hooked_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1blsyn9</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>What am I doing wrong that my DIY manicure doesn't look that clean??</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blsyn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1blsjqm</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>This set took 4-5 hours</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blsjqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1blsdmg</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Went with red for Easter</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cbyps93673qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1bls8ji</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>mastered the cursed nail pose</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fz4p1m4763qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1blrhvw</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt at using polygel with dual forms! Pretty happy with the result </t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z85qrprrz2qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1blreiz</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>just some nails i did</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n27x5z9wy2qc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1blr912</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Magical 🦢</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vh0trhdgx2qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1blr6q5</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Doing my nails at home has saved my natural nails</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blr6q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1blr1e0</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>File down dipped nails</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1byu22dv2qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1blpfim</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>hello! Do you like change?</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blpfim</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1blp6jz</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Hand painted spring nails!</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blp6jz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1bmdd9l</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>First butterfly set!</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3czf127dy7qc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1bmd9l6</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>ILNP- Chai Latte</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bmd9l6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1bmc8dt</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Rose gold?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bmc8dt/rose_gold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1bm9vcb</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Jelliest jelly</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm9vcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1bm9kt5</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Fell in love with tiny dancer through this sub!</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm9kt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1bm7ghd</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Store and display polish</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bm7ghd/store_and_display_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1bm9954</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Spring nails! … except it’s a soggy spring so far over here, so that’s the vibe</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm9954</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1bm93j5</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>1st Mani of Spring 🧡💜</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sdfs6hads6qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1bm8p8w</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>What's a similar lavender shimmery polish thats not out of stock or limited edition</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bm8p8w/whats_a_similar_lavender_shimmery_polish_thats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1bm8jn5</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Essie - Play Date</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm8jn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1bm8i3l</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Help! The bubbles are back!</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bm8i3l/help_the_bubbles_are_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1bm7xs9</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Unique enough?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bm7xs9/unique_enough/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1bm7xob</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Shimmery for Spring🦋</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm7xob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1bm6h2p</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Funhouse topper?</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bm6h2p/funhouse_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1bm7ehj</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cuticle/Nail Skincare help </t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zf3frtdwd6qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1bm74k6</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Help! I got nail polish on my sweater and my brown jeans</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bm74k6/help_i_got_nail_polish_on_my_sweater_and_my_brown/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1bm6vb3</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>In the sun while running errands.</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ymwzock96qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1bm6rvb</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Trying to save a dollar on Dazzle Dry: do I need every step?</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bm6rvb/trying_to_save_a_dollar_on_dazzle_dry_do_i_need/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1bm6nhk</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>🦋 butterfly in the sky ☁️</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm6nhk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1bm6dxz</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Loving this rub on powder 🙂</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om9drb8q56qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1bm6bvb</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Velvet hack comparisons </t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lslrjsc956qc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1bm4wex</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>My first Cirque Jellies</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm4wex</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1bm5wkb</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Makin' my way downtown...</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm5wkb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1bm5b2m</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Cuticle Nipper Recs?</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bm5b2m/cuticle_nipper_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1bm58yy</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>DAE constantly stares at their polish collection?🥲</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bm58yy/dae_constantly_stares_at_their_polish_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1bm4uno</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question about polish comparison between Phoenix and Bees Knees Lacquer. As far as surviving wear and tear- which one lasts longest? </t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bm4uno/question_about_polish_comparison_between_phoenix/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1bm47xy</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>🩵💎Aqua Geode💎🩵</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm47xy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1bm441q</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Nail pics with phone camera</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bm441q/nail_pics_with_phone_camera/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1bm3vv7</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Mooncat midnight Rider &amp; HoH</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wvwol9hdm5qc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1bm3uov</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Let me AXE you a question</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm3uov</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1bm3n5q</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Too chicken to dye my hair copper so copper mani it is 😌</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm3n5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1bm3m1k</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Leftover residue from gel nails?</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm3m1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1bm3ktz</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails keep breaking and not sure what I need. </t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bm3ktz/nails_keep_breaking_and_not_sure_what_i_need/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1bm3evr</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Lyn b swatches on my husband</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm3evr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1bm30iq</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>In love with this combo</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tw4v2niuf5qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1bm2wz9</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Colores de Carol</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4kfps4e2f5qc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1bm2n1a</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is Seche Vite legally allowed to claim this? It's so blatantly false, my nails will start to yellow a couple of days after painting them and using this top coat. </t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbb5dkn2d5qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1bm2g9n</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Celebrate, We Will!</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm2g9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1bm23ay</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Skittles </t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vnoz7wy85qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1bm1xj5</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Sometimes a nice neutral just hits the spot</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kv1ovw6s75qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1bm1vda</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>My fiance and I sporting the new lumen Papillion and Blue Morpho! &amp; Bonus pic showing them with ube jelly base layer, really makes them both pop!</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm1vda</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1bm0fge</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>💐🌷Spring!</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6yq1kfkrw4qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1bm0epq</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Saturday self-manicure 💅</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm0epq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1bm01y9</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Crelly or Jelly recs (besides Cirque) </t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bm01y9/crelly_or_jelly_recs_besides_cirque/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1blzhn1</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Under Cover, Grapes</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tef1fcbvp4qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1blyk94</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>BKL Wyrd Appreciation</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3onph8mxi4qc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1blxuc4</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>You'll Never Take Me Alive, Copper! 😆</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/PVzVRdR</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1blx9kz</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can anyone recommend a lavender or lilac magnetic polish? </t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1blx9kz/can_anyone_recommend_a_lavender_or_lilac_magnetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1blwvxl</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Spring nails!</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6eehovhc64qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1blw840</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Inglorious buzzards is so much fun, and feels appropriate for a desert adventure.</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blw840</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1blvf4d</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Blue/purple glow in the dark recs</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1blvf4d/bluepurple_glow_in_the_dark_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1blv8dg</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Why do these dry so differently?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4r09gxyt3qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1bltxt1</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>transparent micro holographic topper recs?</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bltxt1/transparent_micro_holographic_topper_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1blth6a</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>On Saturdays I wear pink</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rq9ksu8cg3qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1blsq7g</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>I love how fun these neon colors look! And a little splash of green for March 🍀</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blsq7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1blsoy3</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Cirque restock? (jellies)</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1blsoy3/cirque_restock_jellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1blsj35</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>ILNP - yes please</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blsj35</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1blsdwx</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Did my nails with Ohora - N Addict</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8v8lp7h573qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1blsc5k</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Grade School Crush by Pop Arazzi</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blsc5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1bls2ez</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Lynb Jackie Daytona regular human bartender</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bls2ez</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1bls05o</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>First two attempts at stamping</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bls05o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1blrk4l</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Rogue and their always-wild flakies 😍</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z97u6gad03qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1blrcgj</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>So in love with this polish</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blrcgj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1blgegy</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Jelly layering 🍒</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blgegy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1blpwwq</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Fancy Gloss Blue Speckled Egg, Seche Vite, no base coat</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wivyj78j2qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1bln8cj</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Cherry blossom (&amp; question about acrylic paint)</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibmjskoym1qc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1bmbqyo</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Solar Eclipse nails! Credit @muiibailey on IG, the best nail tech in Vegas. </t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/av5j6mx6h7qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1bmalak</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Nail Tutorial | Flower Design 🌸 🌺  | Long Coffin Tips</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://youtu.be/HV8eOJdC2nk?si=W5zqNrWnp6BqC7p8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1bm8d5j</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Birthday set</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm8d5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1bm5bnm</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Badass Spring Princess Vibes 👸</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdu756vgx5qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1bm3k4t</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painted this set today 🍓 </t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0yli3nwj5qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1bm28lf</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Fire idea, garbage execution</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm28lf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1bm1rk7</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made a BTS theme press on set </t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/su8jj3ek65qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1bm09dr</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>How do you rate my work? 🫶🏻🌸</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bm09dr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1blz2ct</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>I've just started figuring out how to do my nails, and these are the first two designs I did!</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blz2ct</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1blyqe6</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Matching sets</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1blyqe6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1blwbdj</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Made my first press on set !</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/npya5fl124qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1blvobu</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Feeling like a fairy in a whimsical garden with my new nails 🧚‍♀️🍄</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4ayuki7x3qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1blqtrl</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>It’s giving Buffy 🪵🗡️</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jzpzxbf3t2qc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1blpw16</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Hot mess by me 🔥</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckh6dse1j2qc1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>